<commit_message>
Minor modifications to text messages (2)
</commit_message>
<xml_diff>
--- a/osiris/Documentation/Ping_Failure_Message_Glossary.xlsx
+++ b/osiris/Documentation/Ping_Failure_Message_Glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goorrob\Documents\GitHub\osiris\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A87CB7A0-FF64-4021-9E9B-999B83CE8471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B837F9FE-9C8A-4B04-9A75-9CE56A9AC764}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="4125" windowWidth="28800" windowHeight="15435" xr2:uid="{A226AE24-A6A6-4452-B12A-847F8A89D7E9}"/>
+    <workbookView xWindow="7350" yWindow="1785" windowWidth="28800" windowHeight="17400" xr2:uid="{A226AE24-A6A6-4452-B12A-847F8A89D7E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
   <si>
     <t>Message Number</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Could not find named marker set</t>
   </si>
   <si>
-    <t>Could not locus to set locus-specific threshold</t>
-  </si>
-  <si>
     <t>Could not load MessageBook:  could not find sample level</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>Sample has one or more channels with no data for fragment analysis</t>
   </si>
   <si>
-    <t>Sample is not a valid fsa/hid file for fragment analysis</t>
-  </si>
-  <si>
     <t>Sample caused unexpected crash for fragment analysis</t>
   </si>
   <si>
@@ -235,6 +229,9 @@
   </si>
   <si>
     <t>Version</t>
+  </si>
+  <si>
+    <t>Could not set locus-specific threshold</t>
   </si>
 </sst>
 </file>
@@ -632,7 +629,7 @@
   <dimension ref="A1:D638"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -647,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -685,7 +682,7 @@
         <v>2.15</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -697,7 +694,7 @@
         <v>2.15</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -709,7 +706,7 @@
         <v>2.15</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="4"/>
     </row>
@@ -721,7 +718,7 @@
         <v>2.15</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -733,7 +730,7 @@
         <v>2.15</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="4"/>
     </row>
@@ -745,7 +742,7 @@
         <v>2.15</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="4"/>
     </row>
@@ -757,7 +754,7 @@
         <v>2.15</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="4"/>
     </row>
@@ -769,7 +766,7 @@
         <v>2.15</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="4"/>
     </row>
@@ -781,7 +778,7 @@
         <v>2.15</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="4"/>
     </row>
@@ -793,7 +790,7 @@
         <v>2.15</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="4"/>
     </row>
@@ -805,7 +802,7 @@
         <v>2.15</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="4"/>
     </row>
@@ -817,7 +814,7 @@
         <v>2.15</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="4"/>
     </row>
@@ -829,7 +826,7 @@
         <v>2.15</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="4"/>
     </row>
@@ -841,7 +838,7 @@
         <v>2.15</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="4"/>
     </row>
@@ -853,7 +850,7 @@
         <v>2.15</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="4"/>
     </row>
@@ -865,7 +862,7 @@
         <v>2.15</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="4"/>
     </row>
@@ -877,7 +874,7 @@
         <v>2.15</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="4"/>
     </row>
@@ -889,7 +886,7 @@
         <v>2.15</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D22" s="4"/>
     </row>
@@ -901,7 +898,7 @@
         <v>2.15</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="4"/>
     </row>
@@ -913,7 +910,7 @@
         <v>2.15</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" s="4"/>
     </row>
@@ -925,7 +922,7 @@
         <v>2.15</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" s="4"/>
     </row>
@@ -937,7 +934,7 @@
         <v>2.15</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" s="4"/>
     </row>
@@ -949,7 +946,7 @@
         <v>2.15</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" s="4"/>
     </row>
@@ -961,7 +958,7 @@
         <v>2.15</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D28" s="4"/>
     </row>
@@ -973,7 +970,7 @@
         <v>2.15</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" s="4"/>
     </row>
@@ -985,7 +982,7 @@
         <v>2.15</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D30" s="4"/>
     </row>
@@ -997,7 +994,7 @@
         <v>2.15</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" s="4"/>
     </row>
@@ -1009,7 +1006,7 @@
         <v>2.15</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="4"/>
     </row>
@@ -1021,7 +1018,7 @@
         <v>2.15</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" s="4"/>
     </row>
@@ -1033,7 +1030,7 @@
         <v>2.15</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" s="4"/>
     </row>
@@ -1045,7 +1042,7 @@
         <v>2.15</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D35" s="4"/>
     </row>
@@ -1057,7 +1054,7 @@
         <v>2.15</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="4"/>
     </row>
@@ -1069,7 +1066,7 @@
         <v>2.15</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" s="4"/>
     </row>
@@ -1081,7 +1078,7 @@
         <v>2.15</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" s="4"/>
     </row>
@@ -1093,7 +1090,7 @@
         <v>2.15</v>
       </c>
       <c r="C39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D39" s="4"/>
     </row>
@@ -1105,7 +1102,7 @@
         <v>2.15</v>
       </c>
       <c r="C40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D40" s="4"/>
     </row>
@@ -1129,7 +1126,7 @@
         <v>2.15</v>
       </c>
       <c r="C42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D42" s="4"/>
     </row>
@@ -1141,7 +1138,7 @@
         <v>2.15</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D43" s="4"/>
     </row>
@@ -1153,7 +1150,7 @@
         <v>2.15</v>
       </c>
       <c r="C44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D44" s="4"/>
     </row>
@@ -1165,7 +1162,7 @@
         <v>2.15</v>
       </c>
       <c r="C45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D45" s="4"/>
     </row>
@@ -1177,7 +1174,7 @@
         <v>2.15</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D46" s="4"/>
     </row>
@@ -1189,7 +1186,7 @@
         <v>2.15</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D47" s="4"/>
     </row>
@@ -1201,7 +1198,7 @@
         <v>2.15</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D48" s="4"/>
     </row>
@@ -1213,7 +1210,7 @@
         <v>2.15</v>
       </c>
       <c r="C49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D49" s="4"/>
     </row>
@@ -1225,7 +1222,7 @@
         <v>2.15</v>
       </c>
       <c r="C50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D50" s="4"/>
     </row>
@@ -1237,7 +1234,7 @@
         <v>2.15</v>
       </c>
       <c r="C51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D51" s="4"/>
     </row>
@@ -1249,7 +1246,7 @@
         <v>2.15</v>
       </c>
       <c r="C52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D52" s="4"/>
     </row>
@@ -1261,7 +1258,7 @@
         <v>2.15</v>
       </c>
       <c r="C53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D53" s="4"/>
     </row>
@@ -1273,7 +1270,7 @@
         <v>2.15</v>
       </c>
       <c r="C54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D54" s="4"/>
     </row>
@@ -1285,7 +1282,7 @@
         <v>2.15</v>
       </c>
       <c r="C55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D55" s="4"/>
     </row>
@@ -1297,7 +1294,7 @@
         <v>2.15</v>
       </c>
       <c r="C56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D56" s="4"/>
     </row>
@@ -1309,7 +1306,7 @@
         <v>2.15</v>
       </c>
       <c r="C57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D57" s="4"/>
     </row>
@@ -1321,7 +1318,7 @@
         <v>2.15</v>
       </c>
       <c r="C58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D58" s="4"/>
     </row>
@@ -1333,7 +1330,7 @@
         <v>2.15</v>
       </c>
       <c r="C59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D59" s="4"/>
     </row>
@@ -1345,7 +1342,7 @@
         <v>2.15</v>
       </c>
       <c r="C60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D60" s="4"/>
     </row>
@@ -1357,7 +1354,7 @@
         <v>2.15</v>
       </c>
       <c r="C61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D61" s="4"/>
     </row>
@@ -1369,7 +1366,7 @@
         <v>2.15</v>
       </c>
       <c r="C62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D62" s="4"/>
     </row>
@@ -1381,7 +1378,7 @@
         <v>2.15</v>
       </c>
       <c r="C63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D63" s="4"/>
     </row>
@@ -1393,7 +1390,7 @@
         <v>2.15</v>
       </c>
       <c r="C64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D64" s="4"/>
     </row>
@@ -1405,7 +1402,7 @@
         <v>2.15</v>
       </c>
       <c r="C65" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D65" s="4"/>
     </row>
@@ -1417,7 +1414,7 @@
         <v>2.15</v>
       </c>
       <c r="C66" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D66" s="4"/>
     </row>
@@ -1429,7 +1426,7 @@
         <v>2.15</v>
       </c>
       <c r="C67" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D67" s="4"/>
     </row>
@@ -1441,7 +1438,7 @@
         <v>2.15</v>
       </c>
       <c r="C68" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D68" s="4"/>
     </row>
@@ -1453,7 +1450,7 @@
         <v>2.15</v>
       </c>
       <c r="C69" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D69" s="4"/>
     </row>

</xml_diff>